<commit_message>
[cập nhật tiến độ] Yêu cầu Số 4 từ 90% thành 100%: Đã tạo được Application Context cho 2 function sử dụng, giúp phân biệt từng loại người dùng Mọi người tham khảo để tạo Trigger cho tiện
</commit_message>
<xml_diff>
--- a/bảng phân công bài tập.xlsx
+++ b/bảng phân công bài tập.xlsx
@@ -22,9 +22,6 @@
     <t>Nội dung yêu cầu</t>
   </si>
   <si>
-    <t>Lâm</t>
-  </si>
-  <si>
     <t>Khánh</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>tiến độ</t>
+  </si>
+  <si>
+    <t>Lâm-1412279</t>
   </si>
 </sst>
 </file>
@@ -102,12 +102,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -148,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -160,13 +166,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,14 +483,15 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B8" sqref="B8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="2" max="2" width="50.42578125" customWidth="1"/>
-    <col min="3" max="5" width="9.140625" style="1"/>
+    <col min="3" max="3" width="14.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -492,16 +502,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>21</v>
+      <c r="F1" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -509,14 +519,14 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="6">
+      <c r="F2" s="8">
         <v>1</v>
       </c>
     </row>
@@ -525,14 +535,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="6">
+      <c r="F3" s="8">
         <v>1</v>
       </c>
     </row>
@@ -541,14 +551,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
@@ -556,19 +566,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0.9</v>
+        <v>5</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -576,11 +586,11 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -589,24 +599,24 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>6</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="B8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -614,11 +624,11 @@
         <v>7.1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="3"/>
     </row>
@@ -627,10 +637,10 @@
         <v>7.2</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -640,12 +650,12 @@
         <v>7.3</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -653,11 +663,11 @@
         <v>7.4</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -666,10 +676,10 @@
         <v>7.5</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -678,28 +688,28 @@
       <c r="A14" s="2">
         <v>8</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="B14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>8.1</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -707,16 +717,16 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Cập nhật yêu cầu số 7.3] trưởng chi nhánh Hà Nội có thể xem thông tin dự án chi nhánh khác. Tạo các Label bằng script, chưa tạo bằng function được Các bạn nhớ đánh dấu theo mẫu trong file excel về tiến độ của mỗi yêu cầu nhan
</commit_message>
<xml_diff>
--- a/bảng phân công bài tập.xlsx
+++ b/bảng phân công bài tập.xlsx
@@ -169,13 +169,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:E8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,12 +521,12 @@
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>1</v>
       </c>
     </row>
@@ -537,12 +537,12 @@
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>1</v>
       </c>
     </row>
@@ -568,7 +568,7 @@
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -577,7 +577,7 @@
       <c r="E5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>1</v>
       </c>
     </row>
@@ -611,12 +611,12 @@
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -652,10 +652,13 @@
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3"/>
+      <c r="C11" s="6"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="F11" s="7">
+        <v>0.9</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -688,12 +691,12 @@
       <c r="A14" s="2">
         <v>8</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2">

</xml_diff>

<commit_message>
[Cập nhật tạm thời các file được chia nhỏ ra] Yêu cầu 8.1 bước đầu tạm thời cài đặt như vầy
</commit_message>
<xml_diff>
--- a/bảng phân công bài tập.xlsx
+++ b/bảng phân công bài tập.xlsx
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +658,7 @@
         <v>5</v>
       </c>
       <c r="F11" s="7">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -705,7 +705,7 @@
       <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -713,6 +713,9 @@
       </c>
       <c r="E15" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0.9</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[Cập nhật các File báo cáo] Nội dung báo cáo mình đã phân ra từng file như vầy. Link video youtube nằm trong file README.MD . Có sai sót gì nhớ Alarm liền nha P/S: Nhớ update cái file phân công Excel cho dễ theo dõi nha
</commit_message>
<xml_diff>
--- a/bảng phân công bài tập.xlsx
+++ b/bảng phân công bài tập.xlsx
@@ -482,8 +482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>